<commit_message>
Fix jupyter graphs scripts, load graphs images
</commit_message>
<xml_diff>
--- a/utils/data/pdr_nuvolaPunti.xlsx
+++ b/utils/data/pdr_nuvolaPunti.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="15">
   <si>
     <t>delay</t>
   </si>
@@ -72,6 +72,9 @@
   <si>
     <t>Test1</t>
   </si>
+  <si>
+    <t>mean</t>
+  </si>
 </sst>
 </file>
 
@@ -100,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -123,17 +126,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -668,11 +688,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="252728752"/>
-        <c:axId val="252729144"/>
+        <c:axId val="306960680"/>
+        <c:axId val="306959896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="252728752"/>
+        <c:axId val="306960680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100"/>
@@ -787,13 +807,13 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252729144"/>
+        <c:crossAx val="306959896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252729144"/>
+        <c:axId val="306959896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="89"/>
@@ -908,7 +928,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252728752"/>
+        <c:crossAx val="306960680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1549,16 +1569,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1845,15 +1865,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E19"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1869,8 +1892,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>300</v>
       </c>
@@ -1886,8 +1912,11 @@
       <c r="E2" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>55.277777780000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>300</v>
       </c>
@@ -1903,8 +1932,11 @@
       <c r="E3" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2">
+        <v>55.277777780000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>300</v>
       </c>
@@ -1920,8 +1952,11 @@
       <c r="E4" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>55.277777780000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>500</v>
       </c>
@@ -1937,8 +1972,11 @@
       <c r="E5" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>63.611111110000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>500</v>
       </c>
@@ -1954,8 +1992,11 @@
       <c r="E6" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>63.611111110000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>500</v>
       </c>
@@ -1971,8 +2012,11 @@
       <c r="E7" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="2">
+        <v>63.611111110000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>750</v>
       </c>
@@ -1988,8 +2032,11 @@
       <c r="E8" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>750</v>
       </c>
@@ -2005,8 +2052,11 @@
       <c r="E9" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>750</v>
       </c>
@@ -2022,8 +2072,11 @@
       <c r="E10" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1000</v>
       </c>
@@ -2039,8 +2092,11 @@
       <c r="E11" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="2">
+        <v>83.333333330000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1000</v>
       </c>
@@ -2056,8 +2112,11 @@
       <c r="E12" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="2">
+        <v>83.333333330000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1000</v>
       </c>
@@ -2073,8 +2132,11 @@
       <c r="E13" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="2">
+        <v>83.333333330000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1500</v>
       </c>
@@ -2090,8 +2152,11 @@
       <c r="E14" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="2">
+        <v>84.444444439999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1500</v>
       </c>
@@ -2107,8 +2172,11 @@
       <c r="E15" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="2">
+        <v>84.444444439999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1500</v>
       </c>
@@ -2124,8 +2192,11 @@
       <c r="E16" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="2">
+        <v>84.444444439999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>2000</v>
       </c>
@@ -2141,8 +2212,11 @@
       <c r="E17" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="2">
+        <v>86.388888890000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2000</v>
       </c>
@@ -2158,8 +2232,11 @@
       <c r="E18" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <v>86.388888890000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2000</v>
       </c>
@@ -2174,6 +2251,9 @@
       </c>
       <c r="E19" s="2">
         <v>1.0888888889999999</v>
+      </c>
+      <c r="F19" s="2">
+        <v>86.388888890000004</v>
       </c>
     </row>
   </sheetData>
@@ -2185,15 +2265,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E19"/>
+      <selection activeCell="F2" sqref="F2:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2209,8 +2289,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>300</v>
       </c>
@@ -2226,8 +2309,12 @@
       <c r="E2" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>53.611111110000003</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>300</v>
       </c>
@@ -2243,8 +2330,12 @@
       <c r="E3" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2">
+        <v>53.611111110000003</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>300</v>
       </c>
@@ -2260,8 +2351,12 @@
       <c r="E4" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>53.611111110000003</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>500</v>
       </c>
@@ -2277,8 +2372,12 @@
       <c r="E5" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>56.111111110000003</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>500</v>
       </c>
@@ -2294,8 +2393,12 @@
       <c r="E6" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>56.111111110000003</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>500</v>
       </c>
@@ -2311,8 +2414,12 @@
       <c r="E7" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="2">
+        <v>56.111111110000003</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>750</v>
       </c>
@@ -2328,8 +2435,11 @@
       <c r="E8" s="2">
         <v>2.8809292050000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2">
+        <v>63.888888889999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>750</v>
       </c>
@@ -2345,8 +2455,11 @@
       <c r="E9" s="2">
         <v>2.8809292050000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>63.888888889999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>750</v>
       </c>
@@ -2362,8 +2475,11 @@
       <c r="E10" s="2">
         <v>2.8809292050000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>63.888888889999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1000</v>
       </c>
@@ -2379,8 +2495,11 @@
       <c r="E11" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="2">
+        <v>70.277777779999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1000</v>
       </c>
@@ -2396,8 +2515,11 @@
       <c r="E12" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="2">
+        <v>70.277777779999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1000</v>
       </c>
@@ -2413,8 +2535,11 @@
       <c r="E13" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="2">
+        <v>70.277777779999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1500</v>
       </c>
@@ -2430,8 +2555,11 @@
       <c r="E14" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="2">
+        <v>71.388888890000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1500</v>
       </c>
@@ -2447,8 +2575,11 @@
       <c r="E15" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="2">
+        <v>71.388888890000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1500</v>
       </c>
@@ -2464,8 +2595,11 @@
       <c r="E16" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="2">
+        <v>71.388888890000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>2000</v>
       </c>
@@ -2481,8 +2615,11 @@
       <c r="E17" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="2">
+        <v>71.666666669999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2000</v>
       </c>
@@ -2498,8 +2635,11 @@
       <c r="E18" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <v>71.666666669999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2000</v>
       </c>
@@ -2514,6 +2654,9 @@
       </c>
       <c r="E19" s="2">
         <v>0.94300543969999995</v>
+      </c>
+      <c r="F19" s="2">
+        <v>71.666666669999998</v>
       </c>
     </row>
   </sheetData>
@@ -2523,15 +2666,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E19"/>
+      <selection activeCell="F2" sqref="F2:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2547,8 +2690,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>300</v>
       </c>
@@ -2564,8 +2710,12 @@
       <c r="E2" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>300</v>
       </c>
@@ -2581,8 +2731,12 @@
       <c r="E3" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>300</v>
       </c>
@@ -2598,8 +2752,12 @@
       <c r="E4" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>500</v>
       </c>
@@ -2615,8 +2773,12 @@
       <c r="E5" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>500</v>
       </c>
@@ -2632,8 +2794,12 @@
       <c r="E6" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>500</v>
       </c>
@@ -2649,8 +2815,12 @@
       <c r="E7" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>750</v>
       </c>
@@ -2666,8 +2836,11 @@
       <c r="E8" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2">
+        <v>64.722222220000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>750</v>
       </c>
@@ -2683,8 +2856,11 @@
       <c r="E9" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>64.722222220000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>750</v>
       </c>
@@ -2700,8 +2876,11 @@
       <c r="E10" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>64.722222220000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1000</v>
       </c>
@@ -2717,8 +2896,11 @@
       <c r="E11" s="2">
         <v>1.8860108790000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="2">
+        <v>69.166666669999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1000</v>
       </c>
@@ -2734,8 +2916,11 @@
       <c r="E12" s="2">
         <v>1.8860108790000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="2">
+        <v>69.166666669999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1000</v>
       </c>
@@ -2751,8 +2936,11 @@
       <c r="E13" s="2">
         <v>1.8860108790000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="2">
+        <v>69.166666669999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1500</v>
       </c>
@@ -2768,8 +2956,11 @@
       <c r="E14" s="2">
         <v>2.373178314</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="2">
+        <v>71.111111109999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1500</v>
       </c>
@@ -2785,8 +2976,11 @@
       <c r="E15" s="2">
         <v>2.373178314</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="2">
+        <v>71.111111109999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1500</v>
       </c>
@@ -2802,8 +2996,11 @@
       <c r="E16" s="2">
         <v>2.373178314</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="2">
+        <v>71.111111109999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>2000</v>
       </c>
@@ -2819,8 +3016,11 @@
       <c r="E17" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="2">
+        <v>72.777777779999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2000</v>
       </c>
@@ -2836,8 +3036,11 @@
       <c r="E18" s="2">
         <v>1.0888888889999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <v>72.777777779999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2000</v>
       </c>
@@ -2852,6 +3055,9 @@
       </c>
       <c r="E19" s="2">
         <v>1.0888888889999999</v>
+      </c>
+      <c r="F19" s="2">
+        <v>72.777777779999994</v>
       </c>
     </row>
   </sheetData>
@@ -2861,15 +3067,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E19"/>
+      <selection activeCell="F2" sqref="F2:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2885,8 +3091,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>300</v>
       </c>
@@ -2902,8 +3111,12 @@
       <c r="E2" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>300</v>
       </c>
@@ -2919,8 +3132,12 @@
       <c r="E3" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>300</v>
       </c>
@@ -2936,8 +3153,12 @@
       <c r="E4" s="2">
         <v>1.9630223609999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>500</v>
       </c>
@@ -2953,8 +3174,12 @@
       <c r="E5" s="2">
         <v>1.6333333329999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>55</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>500</v>
       </c>
@@ -2970,8 +3195,12 @@
       <c r="E6" s="2">
         <v>1.6333333329999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>55</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>500</v>
       </c>
@@ -2987,8 +3216,12 @@
       <c r="E7" s="2">
         <v>1.6333333329999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="2">
+        <v>55</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>750</v>
       </c>
@@ -3004,8 +3237,11 @@
       <c r="E8" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2">
+        <v>64.722222220000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>750</v>
       </c>
@@ -3021,8 +3257,11 @@
       <c r="E9" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>64.722222220000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>750</v>
       </c>
@@ -3038,8 +3277,11 @@
       <c r="E10" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>64.722222220000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1000</v>
       </c>
@@ -3055,8 +3297,11 @@
       <c r="E11" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="2">
+        <v>71.111111109999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1000</v>
       </c>
@@ -3072,8 +3317,11 @@
       <c r="E12" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="2">
+        <v>71.111111109999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1000</v>
       </c>
@@ -3089,8 +3337,11 @@
       <c r="E13" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="2">
+        <v>71.111111109999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1500</v>
       </c>
@@ -3106,8 +3357,11 @@
       <c r="E14" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="2">
+        <v>73.055555560000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1500</v>
       </c>
@@ -3123,8 +3377,11 @@
       <c r="E15" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="2">
+        <v>73.055555560000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1500</v>
       </c>
@@ -3140,8 +3397,11 @@
       <c r="E16" s="2">
         <v>1.4404646029999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="2">
+        <v>73.055555560000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>2000</v>
       </c>
@@ -3157,8 +3417,11 @@
       <c r="E17" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="2">
+        <v>73.333333330000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2000</v>
       </c>
@@ -3174,8 +3437,11 @@
       <c r="E18" s="2">
         <v>0.94300543969999995</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <v>73.333333330000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2000</v>
       </c>
@@ -3190,6 +3456,9 @@
       </c>
       <c r="E19" s="2">
         <v>0.94300543969999995</v>
+      </c>
+      <c r="F19" s="2">
+        <v>73.333333330000002</v>
       </c>
     </row>
   </sheetData>
@@ -3199,15 +3468,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F2" sqref="F2:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3223,11 +3492,14 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>300</v>
       </c>
@@ -3243,11 +3515,14 @@
       <c r="E2" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2">
+        <v>53.611111110000003</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>300</v>
       </c>
@@ -3263,11 +3538,14 @@
       <c r="E3" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2">
+        <v>53.611111110000003</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>300</v>
       </c>
@@ -3283,11 +3561,14 @@
       <c r="E4" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2">
+        <v>53.611111110000003</v>
+      </c>
+      <c r="G4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>500</v>
       </c>
@@ -3303,11 +3584,14 @@
       <c r="E5" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2">
+        <v>56.111111110000003</v>
+      </c>
+      <c r="G5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>500</v>
       </c>
@@ -3323,11 +3607,14 @@
       <c r="E6" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2">
+        <v>56.111111110000003</v>
+      </c>
+      <c r="G6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>500</v>
       </c>
@@ -3343,11 +3630,14 @@
       <c r="E7" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2">
+        <v>56.111111110000003</v>
+      </c>
+      <c r="G7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>750</v>
       </c>
@@ -3363,11 +3653,14 @@
       <c r="E8" s="2">
         <v>2.8809292050000002</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2">
+        <v>63.888888889999997</v>
+      </c>
+      <c r="G8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>750</v>
       </c>
@@ -3383,11 +3676,14 @@
       <c r="E9" s="2">
         <v>2.8809292050000002</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2">
+        <v>63.888888889999997</v>
+      </c>
+      <c r="G9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>750</v>
       </c>
@@ -3403,11 +3699,14 @@
       <c r="E10" s="2">
         <v>2.8809292050000002</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2">
+        <v>63.888888889999997</v>
+      </c>
+      <c r="G10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1000</v>
       </c>
@@ -3423,11 +3722,14 @@
       <c r="E11" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2">
+        <v>70.277777779999994</v>
+      </c>
+      <c r="G11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1000</v>
       </c>
@@ -3443,11 +3745,14 @@
       <c r="E12" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2">
+        <v>70.277777779999994</v>
+      </c>
+      <c r="G12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1000</v>
       </c>
@@ -3463,11 +3768,14 @@
       <c r="E13" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2">
+        <v>70.277777779999994</v>
+      </c>
+      <c r="G13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1500</v>
       </c>
@@ -3483,11 +3791,14 @@
       <c r="E14" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2">
+        <v>71.388888890000004</v>
+      </c>
+      <c r="G14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1500</v>
       </c>
@@ -3503,11 +3814,14 @@
       <c r="E15" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2">
+        <v>71.388888890000004</v>
+      </c>
+      <c r="G15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1500</v>
       </c>
@@ -3523,11 +3837,14 @@
       <c r="E16" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2">
+        <v>71.388888890000004</v>
+      </c>
+      <c r="G16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>2000</v>
       </c>
@@ -3543,11 +3860,14 @@
       <c r="E17" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2">
+        <v>71.666666669999998</v>
+      </c>
+      <c r="G17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2000</v>
       </c>
@@ -3563,11 +3883,14 @@
       <c r="E18" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2">
+        <v>71.666666669999998</v>
+      </c>
+      <c r="G18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2000</v>
       </c>
@@ -3583,11 +3906,14 @@
       <c r="E19" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2">
+        <v>71.666666669999998</v>
+      </c>
+      <c r="G19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>300</v>
       </c>
@@ -3603,11 +3929,14 @@
       <c r="E20" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>300</v>
       </c>
@@ -3623,11 +3952,14 @@
       <c r="E21" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>300</v>
       </c>
@@ -3643,11 +3975,14 @@
       <c r="E22" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>500</v>
       </c>
@@ -3663,11 +3998,14 @@
       <c r="E23" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>500</v>
       </c>
@@ -3683,11 +4021,14 @@
       <c r="E24" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>500</v>
       </c>
@@ -3703,11 +4044,14 @@
       <c r="E25" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>750</v>
       </c>
@@ -3723,11 +4067,14 @@
       <c r="E26" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>750</v>
       </c>
@@ -3743,11 +4090,14 @@
       <c r="E27" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>750</v>
       </c>
@@ -3763,11 +4113,14 @@
       <c r="E28" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>1000</v>
       </c>
@@ -3783,11 +4136,14 @@
       <c r="E29" s="2">
         <v>1.8860108790000001</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="G29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>1000</v>
       </c>
@@ -3803,11 +4159,14 @@
       <c r="E30" s="2">
         <v>1.8860108790000001</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="G30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>1000</v>
       </c>
@@ -3823,11 +4182,14 @@
       <c r="E31" s="2">
         <v>1.8860108790000001</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="G31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>1500</v>
       </c>
@@ -3843,11 +4205,14 @@
       <c r="E32" s="2">
         <v>2.373178314</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>1500</v>
       </c>
@@ -3863,11 +4228,14 @@
       <c r="E33" s="2">
         <v>2.373178314</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>1500</v>
       </c>
@@ -3883,11 +4251,14 @@
       <c r="E34" s="2">
         <v>2.373178314</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>2000</v>
       </c>
@@ -3903,11 +4274,14 @@
       <c r="E35" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2">
+        <v>72.777777779999994</v>
+      </c>
+      <c r="G35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>2000</v>
       </c>
@@ -3923,11 +4297,14 @@
       <c r="E36" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2">
+        <v>72.777777779999994</v>
+      </c>
+      <c r="G36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>2000</v>
       </c>
@@ -3943,11 +4320,14 @@
       <c r="E37" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2">
+        <v>72.777777779999994</v>
+      </c>
+      <c r="G37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>300</v>
       </c>
@@ -3963,11 +4343,14 @@
       <c r="E38" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>300</v>
       </c>
@@ -3983,11 +4366,14 @@
       <c r="E39" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>300</v>
       </c>
@@ -4003,11 +4389,14 @@
       <c r="E40" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G40" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>500</v>
       </c>
@@ -4023,11 +4412,14 @@
       <c r="E41" s="2">
         <v>1.6333333329999999</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2">
+        <v>55</v>
+      </c>
+      <c r="G41" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>500</v>
       </c>
@@ -4043,11 +4435,14 @@
       <c r="E42" s="2">
         <v>1.6333333329999999</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2">
+        <v>55</v>
+      </c>
+      <c r="G42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>500</v>
       </c>
@@ -4063,11 +4458,14 @@
       <c r="E43" s="2">
         <v>1.6333333329999999</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2">
+        <v>55</v>
+      </c>
+      <c r="G43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>750</v>
       </c>
@@ -4083,11 +4481,14 @@
       <c r="E44" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G44" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>750</v>
       </c>
@@ -4103,11 +4504,14 @@
       <c r="E45" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>750</v>
       </c>
@@ -4123,11 +4527,14 @@
       <c r="E46" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G46" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>1000</v>
       </c>
@@ -4143,11 +4550,14 @@
       <c r="E47" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G47" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>1000</v>
       </c>
@@ -4163,11 +4573,14 @@
       <c r="E48" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G48" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>1000</v>
       </c>
@@ -4183,11 +4596,14 @@
       <c r="E49" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G49" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>1500</v>
       </c>
@@ -4203,11 +4619,14 @@
       <c r="E50" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="2">
+        <v>73.055555560000002</v>
+      </c>
+      <c r="G50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>1500</v>
       </c>
@@ -4223,11 +4642,14 @@
       <c r="E51" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="2">
+        <v>73.055555560000002</v>
+      </c>
+      <c r="G51" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>1500</v>
       </c>
@@ -4243,11 +4665,14 @@
       <c r="E52" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="2">
+        <v>73.055555560000002</v>
+      </c>
+      <c r="G52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>2000</v>
       </c>
@@ -4263,11 +4688,14 @@
       <c r="E53" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="G53" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>2000</v>
       </c>
@@ -4283,11 +4711,14 @@
       <c r="E54" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="G54" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>2000</v>
       </c>
@@ -4303,7 +4734,10 @@
       <c r="E55" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="G55" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4314,15 +4748,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="6" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4338,101 +4775,104 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" t="s">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>300</v>
       </c>
@@ -4448,11 +4888,14 @@
       <c r="E20" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>300</v>
       </c>
@@ -4468,11 +4911,14 @@
       <c r="E21" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>300</v>
       </c>
@@ -4488,11 +4934,14 @@
       <c r="E22" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>500</v>
       </c>
@@ -4508,11 +4957,14 @@
       <c r="E23" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2">
+        <v>63.611111110000003</v>
+      </c>
+      <c r="G23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>500</v>
       </c>
@@ -4528,11 +4980,14 @@
       <c r="E24" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2">
+        <v>63.611111110000003</v>
+      </c>
+      <c r="G24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>500</v>
       </c>
@@ -4548,11 +5003,14 @@
       <c r="E25" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2">
+        <v>63.611111110000003</v>
+      </c>
+      <c r="G25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>750</v>
       </c>
@@ -4568,11 +5026,14 @@
       <c r="E26" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2">
+        <v>75</v>
+      </c>
+      <c r="G26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>750</v>
       </c>
@@ -4588,11 +5049,14 @@
       <c r="E27" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>750</v>
       </c>
@@ -4608,11 +5072,14 @@
       <c r="E28" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2">
+        <v>75</v>
+      </c>
+      <c r="G28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>1000</v>
       </c>
@@ -4628,11 +5095,14 @@
       <c r="E29" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2">
+        <v>83.333333330000002</v>
+      </c>
+      <c r="G29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>1000</v>
       </c>
@@ -4648,11 +5118,14 @@
       <c r="E30" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2">
+        <v>83.333333330000002</v>
+      </c>
+      <c r="G30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>1000</v>
       </c>
@@ -4668,11 +5141,14 @@
       <c r="E31" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2">
+        <v>83.333333330000002</v>
+      </c>
+      <c r="G31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>1500</v>
       </c>
@@ -4688,11 +5164,14 @@
       <c r="E32" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2">
+        <v>84.444444439999998</v>
+      </c>
+      <c r="G32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>1500</v>
       </c>
@@ -4708,11 +5187,14 @@
       <c r="E33" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2">
+        <v>84.444444439999998</v>
+      </c>
+      <c r="G33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>1500</v>
       </c>
@@ -4728,11 +5210,14 @@
       <c r="E34" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2">
+        <v>84.444444439999998</v>
+      </c>
+      <c r="G34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>2000</v>
       </c>
@@ -4748,11 +5233,14 @@
       <c r="E35" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2">
+        <v>86.388888890000004</v>
+      </c>
+      <c r="G35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>2000</v>
       </c>
@@ -4768,11 +5256,14 @@
       <c r="E36" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2">
+        <v>86.388888890000004</v>
+      </c>
+      <c r="G36" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>2000</v>
       </c>
@@ -4788,11 +5279,14 @@
       <c r="E37" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2">
+        <v>86.388888890000004</v>
+      </c>
+      <c r="G37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>300</v>
       </c>
@@ -4808,11 +5302,14 @@
       <c r="E38" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2">
+        <v>53.611111110000003</v>
+      </c>
+      <c r="G38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>300</v>
       </c>
@@ -4828,11 +5325,14 @@
       <c r="E39" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2">
+        <v>53.611111110000003</v>
+      </c>
+      <c r="G39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>300</v>
       </c>
@@ -4848,11 +5348,14 @@
       <c r="E40" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2">
+        <v>53.611111110000003</v>
+      </c>
+      <c r="G40" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>500</v>
       </c>
@@ -4868,11 +5371,14 @@
       <c r="E41" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2">
+        <v>56.111111110000003</v>
+      </c>
+      <c r="G41" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>500</v>
       </c>
@@ -4888,11 +5394,14 @@
       <c r="E42" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2">
+        <v>56.111111110000003</v>
+      </c>
+      <c r="G42" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>500</v>
       </c>
@@ -4908,11 +5417,14 @@
       <c r="E43" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2">
+        <v>56.111111110000003</v>
+      </c>
+      <c r="G43" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>750</v>
       </c>
@@ -4928,11 +5440,14 @@
       <c r="E44" s="2">
         <v>2.8809292050000002</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="2">
+        <v>63.888888889999997</v>
+      </c>
+      <c r="G44" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>750</v>
       </c>
@@ -4948,11 +5463,14 @@
       <c r="E45" s="2">
         <v>2.8809292050000002</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="2">
+        <v>63.888888889999997</v>
+      </c>
+      <c r="G45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>750</v>
       </c>
@@ -4968,11 +5486,14 @@
       <c r="E46" s="2">
         <v>2.8809292050000002</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2">
+        <v>63.888888889999997</v>
+      </c>
+      <c r="G46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>1000</v>
       </c>
@@ -4988,11 +5509,14 @@
       <c r="E47" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="2">
+        <v>70.277777779999994</v>
+      </c>
+      <c r="G47" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>1000</v>
       </c>
@@ -5008,11 +5532,14 @@
       <c r="E48" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="2">
+        <v>70.277777779999994</v>
+      </c>
+      <c r="G48" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>1000</v>
       </c>
@@ -5028,11 +5555,14 @@
       <c r="E49" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2">
+        <v>70.277777779999994</v>
+      </c>
+      <c r="G49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>1500</v>
       </c>
@@ -5048,11 +5578,14 @@
       <c r="E50" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="2">
+        <v>71.388888890000004</v>
+      </c>
+      <c r="G50" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>1500</v>
       </c>
@@ -5068,11 +5601,14 @@
       <c r="E51" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="2">
+        <v>71.388888890000004</v>
+      </c>
+      <c r="G51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>1500</v>
       </c>
@@ -5088,11 +5624,14 @@
       <c r="E52" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="2">
+        <v>71.388888890000004</v>
+      </c>
+      <c r="G52" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>2000</v>
       </c>
@@ -5108,11 +5647,14 @@
       <c r="E53" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="2">
+        <v>71.666666669999998</v>
+      </c>
+      <c r="G53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>2000</v>
       </c>
@@ -5128,11 +5670,14 @@
       <c r="E54" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="2">
+        <v>71.666666669999998</v>
+      </c>
+      <c r="G54" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>2000</v>
       </c>
@@ -5148,11 +5693,14 @@
       <c r="E55" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2">
+        <v>71.666666669999998</v>
+      </c>
+      <c r="G55" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>300</v>
       </c>
@@ -5168,11 +5716,14 @@
       <c r="E56" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G56" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>300</v>
       </c>
@@ -5188,11 +5739,14 @@
       <c r="E57" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G57" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>300</v>
       </c>
@@ -5208,11 +5762,14 @@
       <c r="E58" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G58" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>500</v>
       </c>
@@ -5228,11 +5785,14 @@
       <c r="E59" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G59" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>500</v>
       </c>
@@ -5248,11 +5808,14 @@
       <c r="E60" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G60" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>500</v>
       </c>
@@ -5268,11 +5831,14 @@
       <c r="E61" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G61" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>750</v>
       </c>
@@ -5288,11 +5854,14 @@
       <c r="E62" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G62" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>750</v>
       </c>
@@ -5308,11 +5877,14 @@
       <c r="E63" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G63" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>750</v>
       </c>
@@ -5328,11 +5900,14 @@
       <c r="E64" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G64" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>1000</v>
       </c>
@@ -5348,11 +5923,14 @@
       <c r="E65" s="2">
         <v>1.8860108790000001</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="G65" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>1000</v>
       </c>
@@ -5368,11 +5946,14 @@
       <c r="E66" s="2">
         <v>1.8860108790000001</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="G66" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>1000</v>
       </c>
@@ -5388,11 +5969,14 @@
       <c r="E67" s="2">
         <v>1.8860108790000001</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="G67" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>1500</v>
       </c>
@@ -5408,11 +5992,14 @@
       <c r="E68" s="2">
         <v>2.373178314</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G68" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>1500</v>
       </c>
@@ -5428,11 +6015,14 @@
       <c r="E69" s="2">
         <v>2.373178314</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G69" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>1500</v>
       </c>
@@ -5448,11 +6038,14 @@
       <c r="E70" s="2">
         <v>2.373178314</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G70" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>2000</v>
       </c>
@@ -5468,11 +6061,14 @@
       <c r="E71" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="2">
+        <v>72.777777779999994</v>
+      </c>
+      <c r="G71" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>2000</v>
       </c>
@@ -5488,11 +6084,14 @@
       <c r="E72" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="2">
+        <v>72.777777779999994</v>
+      </c>
+      <c r="G72" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>2000</v>
       </c>
@@ -5508,11 +6107,14 @@
       <c r="E73" s="2">
         <v>1.0888888889999999</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="2">
+        <v>72.777777779999994</v>
+      </c>
+      <c r="G73" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>300</v>
       </c>
@@ -5528,11 +6130,14 @@
       <c r="E74" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G74" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>300</v>
       </c>
@@ -5548,11 +6153,14 @@
       <c r="E75" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G75" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>300</v>
       </c>
@@ -5568,11 +6176,14 @@
       <c r="E76" s="2">
         <v>1.9630223609999999</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G76" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>500</v>
       </c>
@@ -5588,11 +6199,14 @@
       <c r="E77" s="2">
         <v>1.6333333329999999</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="2">
+        <v>55</v>
+      </c>
+      <c r="G77" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>500</v>
       </c>
@@ -5608,11 +6222,14 @@
       <c r="E78" s="2">
         <v>1.6333333329999999</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="2">
+        <v>55</v>
+      </c>
+      <c r="G78" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>500</v>
       </c>
@@ -5628,11 +6245,14 @@
       <c r="E79" s="2">
         <v>1.6333333329999999</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="2">
+        <v>55</v>
+      </c>
+      <c r="G79" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>750</v>
       </c>
@@ -5648,11 +6268,14 @@
       <c r="E80" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G80" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>750</v>
       </c>
@@ -5668,11 +6291,14 @@
       <c r="E81" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G81" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>750</v>
       </c>
@@ -5688,11 +6314,14 @@
       <c r="E82" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G82" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>1000</v>
       </c>
@@ -5708,11 +6337,14 @@
       <c r="E83" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G83" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>1000</v>
       </c>
@@ -5728,11 +6360,14 @@
       <c r="E84" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G84" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>1000</v>
       </c>
@@ -5748,11 +6383,14 @@
       <c r="E85" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G85" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>1500</v>
       </c>
@@ -5768,11 +6406,14 @@
       <c r="E86" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="2">
+        <v>73.055555560000002</v>
+      </c>
+      <c r="G86" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>1500</v>
       </c>
@@ -5788,11 +6429,14 @@
       <c r="E87" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" s="2">
+        <v>73.055555560000002</v>
+      </c>
+      <c r="G87" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>1500</v>
       </c>
@@ -5808,11 +6452,14 @@
       <c r="E88" s="2">
         <v>1.4404646029999999</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="2">
+        <v>73.055555560000002</v>
+      </c>
+      <c r="G88" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>2000</v>
       </c>
@@ -5828,11 +6475,14 @@
       <c r="E89" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="G89" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>2000</v>
       </c>
@@ -5848,11 +6498,14 @@
       <c r="E90" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="G90" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>2000</v>
       </c>
@@ -5868,7 +6521,10 @@
       <c r="E91" s="2">
         <v>0.94300543969999995</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="G91" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upload PDR acquisitions, Load graphs for test1, allTests, pdr_nuvolaPunt
</commit_message>
<xml_diff>
--- a/utils/data/pdr_nuvolaPunti.xlsx
+++ b/utils/data/pdr_nuvolaPunti.xlsx
@@ -12,12 +12,13 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7830"/>
   </bookViews>
   <sheets>
-    <sheet name="Test2" sheetId="1" r:id="rId1"/>
-    <sheet name="Test3 500ms" sheetId="2" r:id="rId2"/>
-    <sheet name="Test3 5sec" sheetId="3" r:id="rId3"/>
-    <sheet name="Test3 10sec" sheetId="4" r:id="rId4"/>
-    <sheet name="AllTest3" sheetId="5" r:id="rId5"/>
-    <sheet name="AllTests" sheetId="6" r:id="rId6"/>
+    <sheet name="Test1" sheetId="8" r:id="rId1"/>
+    <sheet name="Test2" sheetId="1" r:id="rId2"/>
+    <sheet name="Test3 500ms" sheetId="2" r:id="rId3"/>
+    <sheet name="Test3 5sec" sheetId="3" r:id="rId4"/>
+    <sheet name="Test3 10sec" sheetId="4" r:id="rId5"/>
+    <sheet name="AllTest3" sheetId="5" r:id="rId6"/>
+    <sheet name="AllTests" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="15">
   <si>
     <t>delay</t>
   </si>
@@ -197,7 +198,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Test2!$B$1</c:f>
+              <c:f>Test1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -228,7 +229,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Test2!$A$2:$A$19</c:f>
+              <c:f>Test1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -291,63 +292,63 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Test2!$B$2:$B$19</c:f>
+              <c:f>Test1!$B$2:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>56.666666669999998</c:v>
+                  <c:v>44.166666666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.333333330000002</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.833333330000002</c:v>
+                  <c:v>33.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>50.833333333333336</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>56.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.166666666666671</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.833333333333336</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>62.5</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>63.333333330000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>74.166666669999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>75.833333330000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>82.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>84.166666669999998</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>83.333333330000002</c:v>
+                  <c:v>60.833333333333336</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>83.333333330000002</c:v>
+                  <c:v>61.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>85.833333330000002</c:v>
+                  <c:v>61.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>84.166666669999998</c:v>
+                  <c:v>60.833333333333336</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>85.833333330000002</c:v>
+                  <c:v>60.833333333333336</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>85.833333330000002</c:v>
+                  <c:v>61.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>87.5</c:v>
+                  <c:v>60.833333333333336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,7 +360,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Test2!$C$1</c:f>
+              <c:f>Test1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -390,7 +391,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Test2!$A$2:$A$19</c:f>
+              <c:f>Test1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -453,63 +454,63 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Test2!$C$2:$C$19</c:f>
+              <c:f>Test1!$C$2:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>58.629689030000002</c:v>
+                  <c:v>53.737126619234473</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.296355689999999</c:v>
+                  <c:v>37.070459952567802</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57.796355689999999</c:v>
+                  <c:v>42.903793285901138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.440464599999999</c:v>
+                  <c:v>55.67246140498294</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63.940464599999999</c:v>
+                  <c:v>61.505794738316268</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64.773797939999994</c:v>
+                  <c:v>64.005794738316268</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75.109672110000005</c:v>
+                  <c:v>61.088888888888889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75.943005439999993</c:v>
+                  <c:v>62.75555555555556</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>76.776338769999995</c:v>
+                  <c:v>61.088888888888889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>83.443005439999993</c:v>
+                  <c:v>61.922222222222224</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>85.109672110000005</c:v>
+                  <c:v>63.588888888888889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>84.276338769999995</c:v>
+                  <c:v>61.922222222222224</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84.773797939999994</c:v>
+                  <c:v>62.211111111111116</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>87.273797939999994</c:v>
+                  <c:v>62.211111111111116</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>85.607131269999996</c:v>
+                  <c:v>61.37777777777778</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>86.922222219999995</c:v>
+                  <c:v>61.37777777777778</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>86.922222219999995</c:v>
+                  <c:v>62.211111111111116</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>88.588888890000007</c:v>
+                  <c:v>61.37777777777778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -521,7 +522,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Test2!$D$1</c:f>
+              <c:f>Test1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -554,7 +555,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Test2!$A$2:$A$19</c:f>
+              <c:f>Test1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -617,63 +618,63 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Test2!$D$2:$D$19</c:f>
+              <c:f>Test1!$D$2:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>54.703644310000001</c:v>
+                  <c:v>34.596206714098869</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.370310969999998</c:v>
+                  <c:v>17.929540047432198</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.870310969999998</c:v>
+                  <c:v>23.762873380765534</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63.559535400000001</c:v>
+                  <c:v>45.994205261683732</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61.059535400000001</c:v>
+                  <c:v>51.827538595017074</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61.892868730000004</c:v>
+                  <c:v>54.327538595017074</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73.223661230000005</c:v>
+                  <c:v>58.911111111111111</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74.056994560000007</c:v>
+                  <c:v>60.577777777777783</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74.890327889999995</c:v>
+                  <c:v>58.911111111111111</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81.556994560000007</c:v>
+                  <c:v>59.744444444444447</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>83.223661230000005</c:v>
+                  <c:v>61.411111111111111</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>82.390327889999995</c:v>
+                  <c:v>59.744444444444447</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>81.892868730000004</c:v>
+                  <c:v>61.122222222222227</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>84.392868730000004</c:v>
+                  <c:v>61.122222222222227</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>82.726202060000006</c:v>
+                  <c:v>60.288888888888891</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>84.744444439999995</c:v>
+                  <c:v>60.288888888888891</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>84.744444439999995</c:v>
+                  <c:v>61.122222222222227</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>86.411111109999993</c:v>
+                  <c:v>60.288888888888891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -688,11 +689,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="306960680"/>
-        <c:axId val="306959896"/>
+        <c:axId val="364898112"/>
+        <c:axId val="364895368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="306960680"/>
+        <c:axId val="364898112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100"/>
@@ -807,17 +808,17 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306959896"/>
+        <c:crossAx val="364895368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="306959896"/>
+        <c:axId val="364895368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="89"/>
-          <c:min val="50"/>
+          <c:max val="65"/>
+          <c:min val="25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -856,7 +857,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="it-IT"/>
-                  <a:t>latency (s)</a:t>
+                  <a:t>PDR (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -928,7 +929,844 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306960680"/>
+        <c:crossAx val="364898112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Test2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PDR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Test2!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Test2!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>56.666666669999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.833333330000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.166666669999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>75.833333330000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>84.166666669999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>83.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85.833333330000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>84.166666669999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>85.833333330000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85.833333330000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>87.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Test2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="6350">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Test2!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Test2!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>58.629689030000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.296355689999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.796355689999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66.440464599999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.940464599999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.773797939999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75.109672110000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75.943005439999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76.776338769999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>83.443005439999993</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.109672110000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>84.276338769999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>84.773797939999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>87.273797939999994</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85.607131269999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>86.922222219999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>86.922222219999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.588888890000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Test2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Test2!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Test2!$D$2:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>54.703644310000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.370310969999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.870310969999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.559535400000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.059535400000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61.892868730000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73.223661230000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74.056994560000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74.890327889999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>81.556994560000007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83.223661230000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>82.390327889999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>81.892868730000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>84.392868730000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>82.726202060000006</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>84.744444439999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>84.744444439999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>86.411111109999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="260637256"/>
+        <c:axId val="260631376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="260637256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2100"/>
+          <c:min val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Time between pkt sent (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="260631376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="260631376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="89"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>PDR (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="260637256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1010,6 +1848,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1565,7 +2443,560 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1868,7 +3299,403 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>300</v>
+      </c>
+      <c r="B2">
+        <v>44.166666666666671</v>
+      </c>
+      <c r="C2">
+        <v>53.737126619234473</v>
+      </c>
+      <c r="D2">
+        <v>34.596206714098869</v>
+      </c>
+      <c r="E2">
+        <v>9.5704599525678002</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>300</v>
+      </c>
+      <c r="B3">
+        <v>27.5</v>
+      </c>
+      <c r="C3">
+        <v>37.070459952567802</v>
+      </c>
+      <c r="D3">
+        <v>17.929540047432198</v>
+      </c>
+      <c r="E3">
+        <v>9.5704599525678002</v>
+      </c>
+      <c r="F3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="C4">
+        <v>42.903793285901138</v>
+      </c>
+      <c r="D4">
+        <v>23.762873380765534</v>
+      </c>
+      <c r="E4">
+        <v>9.5704599525678002</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>500</v>
+      </c>
+      <c r="B5">
+        <v>50.833333333333336</v>
+      </c>
+      <c r="C5">
+        <v>55.67246140498294</v>
+      </c>
+      <c r="D5">
+        <v>45.994205261683732</v>
+      </c>
+      <c r="E5">
+        <v>4.8391280716496006</v>
+      </c>
+      <c r="F5">
+        <v>55.555555555555564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>500</v>
+      </c>
+      <c r="B6">
+        <v>56.666666666666671</v>
+      </c>
+      <c r="C6">
+        <v>61.505794738316268</v>
+      </c>
+      <c r="D6">
+        <v>51.827538595017074</v>
+      </c>
+      <c r="E6">
+        <v>4.8391280716496006</v>
+      </c>
+      <c r="F6">
+        <v>55.555555555555564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>500</v>
+      </c>
+      <c r="B7">
+        <v>59.166666666666671</v>
+      </c>
+      <c r="C7">
+        <v>64.005794738316268</v>
+      </c>
+      <c r="D7">
+        <v>54.327538595017074</v>
+      </c>
+      <c r="E7">
+        <v>4.8391280716496006</v>
+      </c>
+      <c r="F7">
+        <v>55.555555555555564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>750</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>61.088888888888889</v>
+      </c>
+      <c r="D8">
+        <v>58.911111111111111</v>
+      </c>
+      <c r="E8">
+        <v>1.0888888888888919</v>
+      </c>
+      <c r="F8">
+        <v>60.555555555555564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>750</v>
+      </c>
+      <c r="B9">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C9">
+        <v>62.75555555555556</v>
+      </c>
+      <c r="D9">
+        <v>60.577777777777783</v>
+      </c>
+      <c r="E9">
+        <v>1.0888888888888919</v>
+      </c>
+      <c r="F9">
+        <v>60.555555555555564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>750</v>
+      </c>
+      <c r="B10">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>61.088888888888889</v>
+      </c>
+      <c r="D10">
+        <v>58.911111111111111</v>
+      </c>
+      <c r="E10">
+        <v>1.0888888888888919</v>
+      </c>
+      <c r="F10">
+        <v>60.555555555555564</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B11">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C11">
+        <v>61.922222222222224</v>
+      </c>
+      <c r="D11">
+        <v>59.744444444444447</v>
+      </c>
+      <c r="E11">
+        <v>1.0888888888888875</v>
+      </c>
+      <c r="F11">
+        <v>61.388888888888893</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>62.5</v>
+      </c>
+      <c r="C12">
+        <v>63.588888888888889</v>
+      </c>
+      <c r="D12">
+        <v>61.411111111111111</v>
+      </c>
+      <c r="E12">
+        <v>1.0888888888888875</v>
+      </c>
+      <c r="F12">
+        <v>61.388888888888893</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B13">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C13">
+        <v>61.922222222222224</v>
+      </c>
+      <c r="D13">
+        <v>59.744444444444447</v>
+      </c>
+      <c r="E13">
+        <v>1.0888888888888875</v>
+      </c>
+      <c r="F13">
+        <v>61.388888888888893</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B14">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C14">
+        <v>62.211111111111116</v>
+      </c>
+      <c r="D14">
+        <v>61.122222222222227</v>
+      </c>
+      <c r="E14">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F14">
+        <v>61.388888888888893</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B15">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C15">
+        <v>62.211111111111116</v>
+      </c>
+      <c r="D15">
+        <v>61.122222222222227</v>
+      </c>
+      <c r="E15">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F15">
+        <v>61.388888888888893</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B16">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C16">
+        <v>61.37777777777778</v>
+      </c>
+      <c r="D16">
+        <v>60.288888888888891</v>
+      </c>
+      <c r="E16">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F16">
+        <v>61.388888888888893</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B17">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C17">
+        <v>61.37777777777778</v>
+      </c>
+      <c r="D17">
+        <v>60.288888888888891</v>
+      </c>
+      <c r="E17">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F17">
+        <v>61.111111111111114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B18">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C18">
+        <v>62.211111111111116</v>
+      </c>
+      <c r="D18">
+        <v>61.122222222222227</v>
+      </c>
+      <c r="E18">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F18">
+        <v>61.111111111111114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B19">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C19">
+        <v>61.37777777777778</v>
+      </c>
+      <c r="D19">
+        <v>60.288888888888891</v>
+      </c>
+      <c r="E19">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F19">
+        <v>61.111111111111114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,12 +4090,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F19"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,407 +4484,6 @@
       </c>
       <c r="F19" s="2">
         <v>71.666666669999998</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>300</v>
-      </c>
-      <c r="B2" s="2">
-        <v>53.333333330000002</v>
-      </c>
-      <c r="C2" s="2">
-        <v>54.422222220000002</v>
-      </c>
-      <c r="D2" s="2">
-        <v>52.244444440000002</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.0888888889999999</v>
-      </c>
-      <c r="F2" s="2">
-        <v>52.777777780000001</v>
-      </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>300</v>
-      </c>
-      <c r="B3" s="2">
-        <v>51.666666669999998</v>
-      </c>
-      <c r="C3" s="2">
-        <v>52.755555559999998</v>
-      </c>
-      <c r="D3" s="2">
-        <v>50.577777779999998</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0888888889999999</v>
-      </c>
-      <c r="F3" s="2">
-        <v>52.777777780000001</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>300</v>
-      </c>
-      <c r="B4" s="2">
-        <v>53.333333330000002</v>
-      </c>
-      <c r="C4" s="2">
-        <v>54.422222220000002</v>
-      </c>
-      <c r="D4" s="2">
-        <v>52.244444440000002</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.0888888889999999</v>
-      </c>
-      <c r="F4" s="2">
-        <v>52.777777780000001</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>500</v>
-      </c>
-      <c r="B5" s="2">
-        <v>55.833333330000002</v>
-      </c>
-      <c r="C5" s="2">
-        <v>56.922222220000002</v>
-      </c>
-      <c r="D5" s="2">
-        <v>54.744444440000002</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.0888888889999999</v>
-      </c>
-      <c r="F5" s="2">
-        <v>55.277777780000001</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>500</v>
-      </c>
-      <c r="B6" s="2">
-        <v>54.166666669999998</v>
-      </c>
-      <c r="C6" s="2">
-        <v>55.255555559999998</v>
-      </c>
-      <c r="D6" s="2">
-        <v>53.077777779999998</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.0888888889999999</v>
-      </c>
-      <c r="F6" s="2">
-        <v>55.277777780000001</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>500</v>
-      </c>
-      <c r="B7" s="2">
-        <v>55.833333330000002</v>
-      </c>
-      <c r="C7" s="2">
-        <v>56.922222220000002</v>
-      </c>
-      <c r="D7" s="2">
-        <v>54.744444440000002</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.0888888889999999</v>
-      </c>
-      <c r="F7" s="2">
-        <v>55.277777780000001</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>750</v>
-      </c>
-      <c r="B8" s="2">
-        <v>66.666666669999998</v>
-      </c>
-      <c r="C8" s="2">
-        <v>68.629689029999994</v>
-      </c>
-      <c r="D8" s="2">
-        <v>64.703644310000001</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.9630223609999999</v>
-      </c>
-      <c r="F8" s="2">
-        <v>64.722222220000006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>750</v>
-      </c>
-      <c r="B9" s="2">
-        <v>64.166666669999998</v>
-      </c>
-      <c r="C9" s="2">
-        <v>66.129689029999994</v>
-      </c>
-      <c r="D9" s="2">
-        <v>62.203644310000001</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.9630223609999999</v>
-      </c>
-      <c r="F9" s="2">
-        <v>64.722222220000006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>750</v>
-      </c>
-      <c r="B10" s="2">
-        <v>63.333333330000002</v>
-      </c>
-      <c r="C10" s="2">
-        <v>65.296355689999999</v>
-      </c>
-      <c r="D10" s="2">
-        <v>61.370310969999998</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.9630223609999999</v>
-      </c>
-      <c r="F10" s="2">
-        <v>64.722222220000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B11" s="2">
-        <v>67.5</v>
-      </c>
-      <c r="C11" s="2">
-        <v>69.386010880000001</v>
-      </c>
-      <c r="D11" s="2">
-        <v>65.613989119999999</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1.8860108790000001</v>
-      </c>
-      <c r="F11" s="2">
-        <v>69.166666669999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B12" s="2">
-        <v>70.833333330000002</v>
-      </c>
-      <c r="C12" s="2">
-        <v>72.719344210000003</v>
-      </c>
-      <c r="D12" s="2">
-        <v>68.947322450000001</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.8860108790000001</v>
-      </c>
-      <c r="F12" s="2">
-        <v>69.166666669999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B13" s="2">
-        <v>69.166666669999998</v>
-      </c>
-      <c r="C13" s="2">
-        <v>71.052677549999999</v>
-      </c>
-      <c r="D13" s="2">
-        <v>67.280655789999997</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.8860108790000001</v>
-      </c>
-      <c r="F13" s="2">
-        <v>69.166666669999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>1500</v>
-      </c>
-      <c r="B14" s="2">
-        <v>69.166666669999998</v>
-      </c>
-      <c r="C14" s="2">
-        <v>71.539844979999998</v>
-      </c>
-      <c r="D14" s="2">
-        <v>66.793488350000004</v>
-      </c>
-      <c r="E14" s="2">
-        <v>2.373178314</v>
-      </c>
-      <c r="F14" s="2">
-        <v>71.111111109999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>1500</v>
-      </c>
-      <c r="B15" s="2">
-        <v>70.833333330000002</v>
-      </c>
-      <c r="C15" s="2">
-        <v>73.206511649999996</v>
-      </c>
-      <c r="D15" s="2">
-        <v>68.460155020000002</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2.373178314</v>
-      </c>
-      <c r="F15" s="2">
-        <v>71.111111109999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>1500</v>
-      </c>
-      <c r="B16" s="2">
-        <v>73.333333330000002</v>
-      </c>
-      <c r="C16" s="2">
-        <v>75.706511649999996</v>
-      </c>
-      <c r="D16" s="2">
-        <v>70.960155020000002</v>
-      </c>
-      <c r="E16" s="2">
-        <v>2.373178314</v>
-      </c>
-      <c r="F16" s="2">
-        <v>71.111111109999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>2000</v>
-      </c>
-      <c r="B17" s="2">
-        <v>73.333333330000002</v>
-      </c>
-      <c r="C17" s="2">
-        <v>74.422222219999995</v>
-      </c>
-      <c r="D17" s="2">
-        <v>72.244444439999995</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1.0888888889999999</v>
-      </c>
-      <c r="F17" s="2">
-        <v>72.777777779999994</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>2000</v>
-      </c>
-      <c r="B18" s="2">
-        <v>73.333333330000002</v>
-      </c>
-      <c r="C18" s="2">
-        <v>74.422222219999995</v>
-      </c>
-      <c r="D18" s="2">
-        <v>72.244444439999995</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1.0888888889999999</v>
-      </c>
-      <c r="F18" s="2">
-        <v>72.777777779999994</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>2000</v>
-      </c>
-      <c r="B19" s="2">
-        <v>71.666666669999998</v>
-      </c>
-      <c r="C19" s="2">
-        <v>72.755555560000005</v>
-      </c>
-      <c r="D19" s="2">
-        <v>70.577777780000005</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1.0888888889999999</v>
-      </c>
-      <c r="F19" s="2">
-        <v>72.777777779999994</v>
       </c>
     </row>
   </sheetData>
@@ -3100,19 +4526,19 @@
         <v>300</v>
       </c>
       <c r="B2" s="2">
-        <v>50.833333330000002</v>
+        <v>53.333333330000002</v>
       </c>
       <c r="C2" s="2">
-        <v>52.796355689999999</v>
+        <v>54.422222220000002</v>
       </c>
       <c r="D2" s="2">
-        <v>48.870310969999998</v>
+        <v>52.244444440000002</v>
       </c>
       <c r="E2" s="2">
-        <v>1.9630223609999999</v>
+        <v>1.0888888889999999</v>
       </c>
       <c r="F2" s="2">
-        <v>52.222222219999999</v>
+        <v>52.777777780000001</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -3121,19 +4547,19 @@
         <v>300</v>
       </c>
       <c r="B3" s="2">
-        <v>54.166666669999998</v>
+        <v>51.666666669999998</v>
       </c>
       <c r="C3" s="2">
-        <v>56.129689030000002</v>
+        <v>52.755555559999998</v>
       </c>
       <c r="D3" s="2">
-        <v>52.203644310000001</v>
+        <v>50.577777779999998</v>
       </c>
       <c r="E3" s="2">
-        <v>1.9630223609999999</v>
+        <v>1.0888888889999999</v>
       </c>
       <c r="F3" s="2">
-        <v>52.222222219999999</v>
+        <v>52.777777780000001</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -3142,19 +4568,19 @@
         <v>300</v>
       </c>
       <c r="B4" s="2">
-        <v>51.666666669999998</v>
+        <v>53.333333330000002</v>
       </c>
       <c r="C4" s="2">
-        <v>53.629689030000002</v>
+        <v>54.422222220000002</v>
       </c>
       <c r="D4" s="2">
-        <v>49.703644310000001</v>
+        <v>52.244444440000002</v>
       </c>
       <c r="E4" s="2">
-        <v>1.9630223609999999</v>
+        <v>1.0888888889999999</v>
       </c>
       <c r="F4" s="2">
-        <v>52.222222219999999</v>
+        <v>52.777777780000001</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -3163,19 +4589,19 @@
         <v>500</v>
       </c>
       <c r="B5" s="2">
-        <v>54.166666669999998</v>
+        <v>55.833333330000002</v>
       </c>
       <c r="C5" s="2">
-        <v>55.8</v>
+        <v>56.922222220000002</v>
       </c>
       <c r="D5" s="2">
-        <v>52.533333329999998</v>
+        <v>54.744444440000002</v>
       </c>
       <c r="E5" s="2">
-        <v>1.6333333329999999</v>
+        <v>1.0888888889999999</v>
       </c>
       <c r="F5" s="2">
-        <v>55</v>
+        <v>55.277777780000001</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -3187,16 +4613,16 @@
         <v>54.166666669999998</v>
       </c>
       <c r="C6" s="2">
-        <v>55.8</v>
+        <v>55.255555559999998</v>
       </c>
       <c r="D6" s="2">
-        <v>52.533333329999998</v>
+        <v>53.077777779999998</v>
       </c>
       <c r="E6" s="2">
-        <v>1.6333333329999999</v>
+        <v>1.0888888889999999</v>
       </c>
       <c r="F6" s="2">
-        <v>55</v>
+        <v>55.277777780000001</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -3205,19 +4631,19 @@
         <v>500</v>
       </c>
       <c r="B7" s="2">
-        <v>56.666666669999998</v>
+        <v>55.833333330000002</v>
       </c>
       <c r="C7" s="2">
-        <v>58.3</v>
+        <v>56.922222220000002</v>
       </c>
       <c r="D7" s="2">
-        <v>55.033333329999998</v>
+        <v>54.744444440000002</v>
       </c>
       <c r="E7" s="2">
-        <v>1.6333333329999999</v>
+        <v>1.0888888889999999</v>
       </c>
       <c r="F7" s="2">
-        <v>55</v>
+        <v>55.277777780000001</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -3226,16 +4652,16 @@
         <v>750</v>
       </c>
       <c r="B8" s="2">
-        <v>65.833333330000002</v>
+        <v>66.666666669999998</v>
       </c>
       <c r="C8" s="2">
-        <v>67.273797939999994</v>
+        <v>68.629689029999994</v>
       </c>
       <c r="D8" s="2">
-        <v>64.392868730000004</v>
+        <v>64.703644310000001</v>
       </c>
       <c r="E8" s="2">
-        <v>1.4404646029999999</v>
+        <v>1.9630223609999999</v>
       </c>
       <c r="F8" s="2">
         <v>64.722222220000006</v>
@@ -3246,16 +4672,16 @@
         <v>750</v>
       </c>
       <c r="B9" s="2">
-        <v>65</v>
+        <v>64.166666669999998</v>
       </c>
       <c r="C9" s="2">
-        <v>66.440464599999999</v>
+        <v>66.129689029999994</v>
       </c>
       <c r="D9" s="2">
-        <v>63.559535400000001</v>
+        <v>62.203644310000001</v>
       </c>
       <c r="E9" s="2">
-        <v>1.4404646029999999</v>
+        <v>1.9630223609999999</v>
       </c>
       <c r="F9" s="2">
         <v>64.722222220000006</v>
@@ -3269,13 +4695,13 @@
         <v>63.333333330000002</v>
       </c>
       <c r="C10" s="2">
-        <v>64.773797939999994</v>
+        <v>65.296355689999999</v>
       </c>
       <c r="D10" s="2">
-        <v>61.892868730000004</v>
+        <v>61.370310969999998</v>
       </c>
       <c r="E10" s="2">
-        <v>1.4404646029999999</v>
+        <v>1.9630223609999999</v>
       </c>
       <c r="F10" s="2">
         <v>64.722222220000006</v>
@@ -3286,19 +4712,19 @@
         <v>1000</v>
       </c>
       <c r="B11" s="2">
-        <v>70.833333330000002</v>
+        <v>67.5</v>
       </c>
       <c r="C11" s="2">
-        <v>72.273797939999994</v>
+        <v>69.386010880000001</v>
       </c>
       <c r="D11" s="2">
-        <v>69.392868730000004</v>
+        <v>65.613989119999999</v>
       </c>
       <c r="E11" s="2">
-        <v>1.4404646029999999</v>
+        <v>1.8860108790000001</v>
       </c>
       <c r="F11" s="2">
-        <v>71.111111109999996</v>
+        <v>69.166666669999998</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3306,19 +4732,19 @@
         <v>1000</v>
       </c>
       <c r="B12" s="2">
-        <v>70</v>
+        <v>70.833333330000002</v>
       </c>
       <c r="C12" s="2">
-        <v>71.440464599999999</v>
+        <v>72.719344210000003</v>
       </c>
       <c r="D12" s="2">
-        <v>68.559535400000001</v>
+        <v>68.947322450000001</v>
       </c>
       <c r="E12" s="2">
-        <v>1.4404646029999999</v>
+        <v>1.8860108790000001</v>
       </c>
       <c r="F12" s="2">
-        <v>71.111111109999996</v>
+        <v>69.166666669999998</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3326,19 +4752,19 @@
         <v>1000</v>
       </c>
       <c r="B13" s="2">
-        <v>72.5</v>
+        <v>69.166666669999998</v>
       </c>
       <c r="C13" s="2">
-        <v>73.940464599999999</v>
+        <v>71.052677549999999</v>
       </c>
       <c r="D13" s="2">
-        <v>71.059535400000001</v>
+        <v>67.280655789999997</v>
       </c>
       <c r="E13" s="2">
-        <v>1.4404646029999999</v>
+        <v>1.8860108790000001</v>
       </c>
       <c r="F13" s="2">
-        <v>71.111111109999996</v>
+        <v>69.166666669999998</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3346,19 +4772,19 @@
         <v>1500</v>
       </c>
       <c r="B14" s="2">
-        <v>71.666666669999998</v>
+        <v>69.166666669999998</v>
       </c>
       <c r="C14" s="2">
-        <v>73.107131269999996</v>
+        <v>71.539844979999998</v>
       </c>
       <c r="D14" s="2">
-        <v>70.226202060000006</v>
+        <v>66.793488350000004</v>
       </c>
       <c r="E14" s="2">
-        <v>1.4404646029999999</v>
+        <v>2.373178314</v>
       </c>
       <c r="F14" s="2">
-        <v>73.055555560000002</v>
+        <v>71.111111109999996</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3366,19 +4792,19 @@
         <v>1500</v>
       </c>
       <c r="B15" s="2">
-        <v>73.333333330000002</v>
+        <v>70.833333330000002</v>
       </c>
       <c r="C15" s="2">
-        <v>74.773797939999994</v>
+        <v>73.206511649999996</v>
       </c>
       <c r="D15" s="2">
-        <v>71.892868730000004</v>
+        <v>68.460155020000002</v>
       </c>
       <c r="E15" s="2">
-        <v>1.4404646029999999</v>
+        <v>2.373178314</v>
       </c>
       <c r="F15" s="2">
-        <v>73.055555560000002</v>
+        <v>71.111111109999996</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3386,19 +4812,19 @@
         <v>1500</v>
       </c>
       <c r="B16" s="2">
-        <v>74.166666669999998</v>
+        <v>73.333333330000002</v>
       </c>
       <c r="C16" s="2">
-        <v>75.607131269999996</v>
+        <v>75.706511649999996</v>
       </c>
       <c r="D16" s="2">
-        <v>72.726202060000006</v>
+        <v>70.960155020000002</v>
       </c>
       <c r="E16" s="2">
-        <v>1.4404646029999999</v>
+        <v>2.373178314</v>
       </c>
       <c r="F16" s="2">
-        <v>73.055555560000002</v>
+        <v>71.111111109999996</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3406,19 +4832,19 @@
         <v>2000</v>
       </c>
       <c r="B17" s="2">
-        <v>72.5</v>
+        <v>73.333333330000002</v>
       </c>
       <c r="C17" s="2">
-        <v>73.443005439999993</v>
+        <v>74.422222219999995</v>
       </c>
       <c r="D17" s="2">
-        <v>71.556994560000007</v>
+        <v>72.244444439999995</v>
       </c>
       <c r="E17" s="2">
-        <v>0.94300543969999995</v>
+        <v>1.0888888889999999</v>
       </c>
       <c r="F17" s="2">
-        <v>73.333333330000002</v>
+        <v>72.777777779999994</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3429,16 +4855,16 @@
         <v>73.333333330000002</v>
       </c>
       <c r="C18" s="2">
-        <v>74.276338769999995</v>
+        <v>74.422222219999995</v>
       </c>
       <c r="D18" s="2">
-        <v>72.390327889999995</v>
+        <v>72.244444439999995</v>
       </c>
       <c r="E18" s="2">
-        <v>0.94300543969999995</v>
+        <v>1.0888888889999999</v>
       </c>
       <c r="F18" s="2">
-        <v>73.333333330000002</v>
+        <v>72.777777779999994</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3446,19 +4872,19 @@
         <v>2000</v>
       </c>
       <c r="B19" s="2">
-        <v>74.166666669999998</v>
+        <v>71.666666669999998</v>
       </c>
       <c r="C19" s="2">
-        <v>75.109672110000005</v>
+        <v>72.755555560000005</v>
       </c>
       <c r="D19" s="2">
-        <v>73.223661230000005</v>
+        <v>70.577777780000005</v>
       </c>
       <c r="E19" s="2">
-        <v>0.94300543969999995</v>
+        <v>1.0888888889999999</v>
       </c>
       <c r="F19" s="2">
-        <v>73.333333330000002</v>
+        <v>72.777777779999994</v>
       </c>
     </row>
   </sheetData>
@@ -3467,6 +4893,407 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>300</v>
+      </c>
+      <c r="B2" s="2">
+        <v>50.833333330000002</v>
+      </c>
+      <c r="C2" s="2">
+        <v>52.796355689999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>48.870310969999998</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.9630223609999999</v>
+      </c>
+      <c r="F2" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>300</v>
+      </c>
+      <c r="B3" s="2">
+        <v>54.166666669999998</v>
+      </c>
+      <c r="C3" s="2">
+        <v>56.129689030000002</v>
+      </c>
+      <c r="D3" s="2">
+        <v>52.203644310000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.9630223609999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>300</v>
+      </c>
+      <c r="B4" s="2">
+        <v>51.666666669999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>53.629689030000002</v>
+      </c>
+      <c r="D4" s="2">
+        <v>49.703644310000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.9630223609999999</v>
+      </c>
+      <c r="F4" s="2">
+        <v>52.222222219999999</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>500</v>
+      </c>
+      <c r="B5" s="2">
+        <v>54.166666669999998</v>
+      </c>
+      <c r="C5" s="2">
+        <v>55.8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>52.533333329999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.6333333329999999</v>
+      </c>
+      <c r="F5" s="2">
+        <v>55</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>500</v>
+      </c>
+      <c r="B6" s="2">
+        <v>54.166666669999998</v>
+      </c>
+      <c r="C6" s="2">
+        <v>55.8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>52.533333329999998</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.6333333329999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>55</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>500</v>
+      </c>
+      <c r="B7" s="2">
+        <v>56.666666669999998</v>
+      </c>
+      <c r="C7" s="2">
+        <v>58.3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>55.033333329999998</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.6333333329999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>55</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>750</v>
+      </c>
+      <c r="B8" s="2">
+        <v>65.833333330000002</v>
+      </c>
+      <c r="C8" s="2">
+        <v>67.273797939999994</v>
+      </c>
+      <c r="D8" s="2">
+        <v>64.392868730000004</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>64.722222220000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>750</v>
+      </c>
+      <c r="B9" s="2">
+        <v>65</v>
+      </c>
+      <c r="C9" s="2">
+        <v>66.440464599999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>63.559535400000001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>64.722222220000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>750</v>
+      </c>
+      <c r="B10" s="2">
+        <v>63.333333330000002</v>
+      </c>
+      <c r="C10" s="2">
+        <v>64.773797939999994</v>
+      </c>
+      <c r="D10" s="2">
+        <v>61.892868730000004</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F10" s="2">
+        <v>64.722222220000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="2">
+        <v>70.833333330000002</v>
+      </c>
+      <c r="C11" s="2">
+        <v>72.273797939999994</v>
+      </c>
+      <c r="D11" s="2">
+        <v>69.392868730000004</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F11" s="2">
+        <v>71.111111109999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="2">
+        <v>70</v>
+      </c>
+      <c r="C12" s="2">
+        <v>71.440464599999999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>68.559535400000001</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F12" s="2">
+        <v>71.111111109999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B13" s="2">
+        <v>72.5</v>
+      </c>
+      <c r="C13" s="2">
+        <v>73.940464599999999</v>
+      </c>
+      <c r="D13" s="2">
+        <v>71.059535400000001</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>71.111111109999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B14" s="2">
+        <v>71.666666669999998</v>
+      </c>
+      <c r="C14" s="2">
+        <v>73.107131269999996</v>
+      </c>
+      <c r="D14" s="2">
+        <v>70.226202060000006</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F14" s="2">
+        <v>73.055555560000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B15" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="C15" s="2">
+        <v>74.773797939999994</v>
+      </c>
+      <c r="D15" s="2">
+        <v>71.892868730000004</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F15" s="2">
+        <v>73.055555560000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B16" s="2">
+        <v>74.166666669999998</v>
+      </c>
+      <c r="C16" s="2">
+        <v>75.607131269999996</v>
+      </c>
+      <c r="D16" s="2">
+        <v>72.726202060000006</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F16" s="2">
+        <v>73.055555560000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B17" s="2">
+        <v>72.5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>73.443005439999993</v>
+      </c>
+      <c r="D17" s="2">
+        <v>71.556994560000007</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.94300543969999995</v>
+      </c>
+      <c r="F17" s="2">
+        <v>73.333333330000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B18" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="C18" s="2">
+        <v>74.276338769999995</v>
+      </c>
+      <c r="D18" s="2">
+        <v>72.390327889999995</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.94300543969999995</v>
+      </c>
+      <c r="F18" s="2">
+        <v>73.333333330000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B19" s="2">
+        <v>74.166666669999998</v>
+      </c>
+      <c r="C19" s="2">
+        <v>75.109672110000005</v>
+      </c>
+      <c r="D19" s="2">
+        <v>73.223661230000005</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.94300543969999995</v>
+      </c>
+      <c r="F19" s="2">
+        <v>73.333333330000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
@@ -4746,12 +6573,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4782,92 +6609,416 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>300</v>
+      </c>
+      <c r="B2">
+        <v>44.166666666666671</v>
+      </c>
+      <c r="C2">
+        <v>53.737126619234473</v>
+      </c>
+      <c r="D2">
+        <v>34.596206714098869</v>
+      </c>
+      <c r="E2">
+        <v>9.5704599525678002</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>300</v>
+      </c>
+      <c r="B3">
+        <v>27.5</v>
+      </c>
+      <c r="C3">
+        <v>37.070459952567802</v>
+      </c>
+      <c r="D3">
+        <v>17.929540047432198</v>
+      </c>
+      <c r="E3">
+        <v>9.5704599525678002</v>
+      </c>
+      <c r="F3">
+        <v>35</v>
+      </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="C4">
+        <v>42.903793285901138</v>
+      </c>
+      <c r="D4">
+        <v>23.762873380765534</v>
+      </c>
+      <c r="E4">
+        <v>9.5704599525678002</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>500</v>
+      </c>
+      <c r="B5">
+        <v>50.833333333333336</v>
+      </c>
+      <c r="C5">
+        <v>55.67246140498294</v>
+      </c>
+      <c r="D5">
+        <v>45.994205261683732</v>
+      </c>
+      <c r="E5">
+        <v>4.8391280716496006</v>
+      </c>
+      <c r="F5">
+        <v>55.555555555555564</v>
+      </c>
       <c r="G5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>500</v>
+      </c>
+      <c r="B6">
+        <v>56.666666666666671</v>
+      </c>
+      <c r="C6">
+        <v>61.505794738316268</v>
+      </c>
+      <c r="D6">
+        <v>51.827538595017074</v>
+      </c>
+      <c r="E6">
+        <v>4.8391280716496006</v>
+      </c>
+      <c r="F6">
+        <v>55.555555555555564</v>
+      </c>
       <c r="G6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>500</v>
+      </c>
+      <c r="B7">
+        <v>59.166666666666671</v>
+      </c>
+      <c r="C7">
+        <v>64.005794738316268</v>
+      </c>
+      <c r="D7">
+        <v>54.327538595017074</v>
+      </c>
+      <c r="E7">
+        <v>4.8391280716496006</v>
+      </c>
+      <c r="F7">
+        <v>55.555555555555564</v>
+      </c>
       <c r="G7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>750</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>61.088888888888889</v>
+      </c>
+      <c r="D8">
+        <v>58.911111111111111</v>
+      </c>
+      <c r="E8">
+        <v>1.0888888888888919</v>
+      </c>
+      <c r="F8">
+        <v>60.555555555555564</v>
+      </c>
       <c r="G8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>750</v>
+      </c>
+      <c r="B9">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C9">
+        <v>62.75555555555556</v>
+      </c>
+      <c r="D9">
+        <v>60.577777777777783</v>
+      </c>
+      <c r="E9">
+        <v>1.0888888888888919</v>
+      </c>
+      <c r="F9">
+        <v>60.555555555555564</v>
+      </c>
       <c r="G9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>750</v>
+      </c>
+      <c r="B10">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>61.088888888888889</v>
+      </c>
+      <c r="D10">
+        <v>58.911111111111111</v>
+      </c>
+      <c r="E10">
+        <v>1.0888888888888919</v>
+      </c>
+      <c r="F10">
+        <v>60.555555555555564</v>
+      </c>
       <c r="G10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B11">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C11">
+        <v>61.922222222222224</v>
+      </c>
+      <c r="D11">
+        <v>59.744444444444447</v>
+      </c>
+      <c r="E11">
+        <v>1.0888888888888875</v>
+      </c>
+      <c r="F11">
+        <v>61.388888888888893</v>
+      </c>
       <c r="G11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>62.5</v>
+      </c>
+      <c r="C12">
+        <v>63.588888888888889</v>
+      </c>
+      <c r="D12">
+        <v>61.411111111111111</v>
+      </c>
+      <c r="E12">
+        <v>1.0888888888888875</v>
+      </c>
+      <c r="F12">
+        <v>61.388888888888893</v>
+      </c>
       <c r="G12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B13">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C13">
+        <v>61.922222222222224</v>
+      </c>
+      <c r="D13">
+        <v>59.744444444444447</v>
+      </c>
+      <c r="E13">
+        <v>1.0888888888888875</v>
+      </c>
+      <c r="F13">
+        <v>61.388888888888893</v>
+      </c>
       <c r="G13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B14">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C14">
+        <v>62.211111111111116</v>
+      </c>
+      <c r="D14">
+        <v>61.122222222222227</v>
+      </c>
+      <c r="E14">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F14">
+        <v>61.388888888888893</v>
+      </c>
       <c r="G14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B15">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C15">
+        <v>62.211111111111116</v>
+      </c>
+      <c r="D15">
+        <v>61.122222222222227</v>
+      </c>
+      <c r="E15">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F15">
+        <v>61.388888888888893</v>
+      </c>
       <c r="G15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B16">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C16">
+        <v>61.37777777777778</v>
+      </c>
+      <c r="D16">
+        <v>60.288888888888891</v>
+      </c>
+      <c r="E16">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F16">
+        <v>61.388888888888893</v>
+      </c>
       <c r="G16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B17">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C17">
+        <v>61.37777777777778</v>
+      </c>
+      <c r="D17">
+        <v>60.288888888888891</v>
+      </c>
+      <c r="E17">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F17">
+        <v>61.111111111111114</v>
+      </c>
       <c r="G17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B18">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C18">
+        <v>62.211111111111116</v>
+      </c>
+      <c r="D18">
+        <v>61.122222222222227</v>
+      </c>
+      <c r="E18">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F18">
+        <v>61.111111111111114</v>
+      </c>
       <c r="G18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B19">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C19">
+        <v>61.37777777777778</v>
+      </c>
+      <c r="D19">
+        <v>60.288888888888891</v>
+      </c>
+      <c r="E19">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F19">
+        <v>61.111111111111114</v>
+      </c>
       <c r="G19" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
fix notebooks, upload fixed and final graphs, fixed file nuvola_punti
</commit_message>
<xml_diff>
--- a/utils/data/pdr_nuvolaPunti.xlsx
+++ b/utils/data/pdr_nuvolaPunti.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7830" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="8" r:id="rId1"/>
     <sheet name="Test2" sheetId="1" r:id="rId2"/>
-    <sheet name="Test3 500ms" sheetId="2" r:id="rId3"/>
-    <sheet name="Test3 5sec" sheetId="3" r:id="rId4"/>
-    <sheet name="Test3 10sec" sheetId="4" r:id="rId5"/>
+    <sheet name="Test3_500ms" sheetId="2" r:id="rId3"/>
+    <sheet name="Test3_5sec" sheetId="3" r:id="rId4"/>
+    <sheet name="Test3_10sec" sheetId="4" r:id="rId5"/>
     <sheet name="AllTest3" sheetId="5" r:id="rId6"/>
     <sheet name="AllTests" sheetId="6" r:id="rId7"/>
+    <sheet name="AllTest" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="16">
   <si>
     <t>delay</t>
   </si>
@@ -75,6 +76,9 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>Test3</t>
   </si>
 </sst>
 </file>
@@ -689,11 +693,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="364898112"/>
-        <c:axId val="364895368"/>
+        <c:axId val="262350856"/>
+        <c:axId val="262349288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="364898112"/>
+        <c:axId val="262350856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100"/>
@@ -741,7 +745,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -808,13 +811,13 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364895368"/>
+        <c:crossAx val="262349288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="364895368"/>
+        <c:axId val="262349288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65"/>
@@ -862,7 +865,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -929,7 +931,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364898112"/>
+        <c:crossAx val="262350856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -943,7 +945,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1526,11 +1527,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="260637256"/>
-        <c:axId val="260631376"/>
+        <c:axId val="262348896"/>
+        <c:axId val="262349680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="260637256"/>
+        <c:axId val="262348896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2100"/>
@@ -1578,7 +1579,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1645,13 +1645,13 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260631376"/>
+        <c:crossAx val="262349680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="260631376"/>
+        <c:axId val="262349680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="89"/>
@@ -1699,7 +1699,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1766,7 +1765,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260637256"/>
+        <c:crossAx val="262348896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1780,7 +1779,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3298,7 +3296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -4896,8 +4894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6577,8 +6575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8682,4 +8680,1284 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G39" sqref="G39:G55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>300</v>
+      </c>
+      <c r="B2">
+        <v>44.166666666666671</v>
+      </c>
+      <c r="C2">
+        <v>53.737126619234473</v>
+      </c>
+      <c r="D2">
+        <v>34.596206714098869</v>
+      </c>
+      <c r="E2">
+        <v>9.5704599525678002</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>300</v>
+      </c>
+      <c r="B3">
+        <v>27.5</v>
+      </c>
+      <c r="C3">
+        <v>37.070459952567802</v>
+      </c>
+      <c r="D3">
+        <v>17.929540047432198</v>
+      </c>
+      <c r="E3">
+        <v>9.5704599525678002</v>
+      </c>
+      <c r="F3">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="C4">
+        <v>42.903793285901138</v>
+      </c>
+      <c r="D4">
+        <v>23.762873380765534</v>
+      </c>
+      <c r="E4">
+        <v>9.5704599525678002</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>500</v>
+      </c>
+      <c r="B5">
+        <v>50.833333333333336</v>
+      </c>
+      <c r="C5">
+        <v>55.67246140498294</v>
+      </c>
+      <c r="D5">
+        <v>45.994205261683732</v>
+      </c>
+      <c r="E5">
+        <v>4.8391280716496006</v>
+      </c>
+      <c r="F5">
+        <v>55.555555555555564</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>500</v>
+      </c>
+      <c r="B6">
+        <v>56.666666666666671</v>
+      </c>
+      <c r="C6">
+        <v>61.505794738316268</v>
+      </c>
+      <c r="D6">
+        <v>51.827538595017074</v>
+      </c>
+      <c r="E6">
+        <v>4.8391280716496006</v>
+      </c>
+      <c r="F6">
+        <v>55.555555555555564</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>500</v>
+      </c>
+      <c r="B7">
+        <v>59.166666666666671</v>
+      </c>
+      <c r="C7">
+        <v>64.005794738316268</v>
+      </c>
+      <c r="D7">
+        <v>54.327538595017074</v>
+      </c>
+      <c r="E7">
+        <v>4.8391280716496006</v>
+      </c>
+      <c r="F7">
+        <v>55.555555555555564</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>750</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>61.088888888888889</v>
+      </c>
+      <c r="D8">
+        <v>58.911111111111111</v>
+      </c>
+      <c r="E8">
+        <v>1.0888888888888919</v>
+      </c>
+      <c r="F8">
+        <v>60.555555555555564</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>750</v>
+      </c>
+      <c r="B9">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C9">
+        <v>62.75555555555556</v>
+      </c>
+      <c r="D9">
+        <v>60.577777777777783</v>
+      </c>
+      <c r="E9">
+        <v>1.0888888888888919</v>
+      </c>
+      <c r="F9">
+        <v>60.555555555555564</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>750</v>
+      </c>
+      <c r="B10">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>61.088888888888889</v>
+      </c>
+      <c r="D10">
+        <v>58.911111111111111</v>
+      </c>
+      <c r="E10">
+        <v>1.0888888888888919</v>
+      </c>
+      <c r="F10">
+        <v>60.555555555555564</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B11">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C11">
+        <v>61.922222222222224</v>
+      </c>
+      <c r="D11">
+        <v>59.744444444444447</v>
+      </c>
+      <c r="E11">
+        <v>1.0888888888888875</v>
+      </c>
+      <c r="F11">
+        <v>61.388888888888893</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>62.5</v>
+      </c>
+      <c r="C12">
+        <v>63.588888888888889</v>
+      </c>
+      <c r="D12">
+        <v>61.411111111111111</v>
+      </c>
+      <c r="E12">
+        <v>1.0888888888888875</v>
+      </c>
+      <c r="F12">
+        <v>61.388888888888893</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B13">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C13">
+        <v>61.922222222222224</v>
+      </c>
+      <c r="D13">
+        <v>59.744444444444447</v>
+      </c>
+      <c r="E13">
+        <v>1.0888888888888875</v>
+      </c>
+      <c r="F13">
+        <v>61.388888888888893</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B14">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C14">
+        <v>62.211111111111116</v>
+      </c>
+      <c r="D14">
+        <v>61.122222222222227</v>
+      </c>
+      <c r="E14">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F14">
+        <v>61.388888888888893</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B15">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C15">
+        <v>62.211111111111116</v>
+      </c>
+      <c r="D15">
+        <v>61.122222222222227</v>
+      </c>
+      <c r="E15">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F15">
+        <v>61.388888888888893</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B16">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C16">
+        <v>61.37777777777778</v>
+      </c>
+      <c r="D16">
+        <v>60.288888888888891</v>
+      </c>
+      <c r="E16">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F16">
+        <v>61.388888888888893</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B17">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C17">
+        <v>61.37777777777778</v>
+      </c>
+      <c r="D17">
+        <v>60.288888888888891</v>
+      </c>
+      <c r="E17">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F17">
+        <v>61.111111111111114</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B18">
+        <v>61.666666666666671</v>
+      </c>
+      <c r="C18">
+        <v>62.211111111111116</v>
+      </c>
+      <c r="D18">
+        <v>61.122222222222227</v>
+      </c>
+      <c r="E18">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F18">
+        <v>61.111111111111114</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B19">
+        <v>60.833333333333336</v>
+      </c>
+      <c r="C19">
+        <v>61.37777777777778</v>
+      </c>
+      <c r="D19">
+        <v>60.288888888888891</v>
+      </c>
+      <c r="E19">
+        <v>0.54444444444444595</v>
+      </c>
+      <c r="F19">
+        <v>61.111111111111114</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>300</v>
+      </c>
+      <c r="B20" s="2">
+        <v>56.666666669999998</v>
+      </c>
+      <c r="C20" s="2">
+        <v>58.629689030000002</v>
+      </c>
+      <c r="D20" s="2">
+        <v>54.703644310000001</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.9630223609999999</v>
+      </c>
+      <c r="F20" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>300</v>
+      </c>
+      <c r="B21" s="2">
+        <v>53.333333330000002</v>
+      </c>
+      <c r="C21" s="2">
+        <v>55.296355689999999</v>
+      </c>
+      <c r="D21" s="2">
+        <v>51.370310969999998</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.9630223609999999</v>
+      </c>
+      <c r="F21" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>300</v>
+      </c>
+      <c r="B22" s="2">
+        <v>55.833333330000002</v>
+      </c>
+      <c r="C22" s="2">
+        <v>57.796355689999999</v>
+      </c>
+      <c r="D22" s="2">
+        <v>53.870310969999998</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.9630223609999999</v>
+      </c>
+      <c r="F22" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>500</v>
+      </c>
+      <c r="B23" s="2">
+        <v>65</v>
+      </c>
+      <c r="C23" s="2">
+        <v>66.440464599999999</v>
+      </c>
+      <c r="D23" s="2">
+        <v>63.559535400000001</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>63.611111110000003</v>
+      </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>500</v>
+      </c>
+      <c r="B24" s="2">
+        <v>62.5</v>
+      </c>
+      <c r="C24" s="2">
+        <v>63.940464599999999</v>
+      </c>
+      <c r="D24" s="2">
+        <v>61.059535400000001</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F24" s="2">
+        <v>63.611111110000003</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>500</v>
+      </c>
+      <c r="B25" s="2">
+        <v>63.333333330000002</v>
+      </c>
+      <c r="C25" s="2">
+        <v>64.773797939999994</v>
+      </c>
+      <c r="D25" s="2">
+        <v>61.892868730000004</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F25" s="2">
+        <v>63.611111110000003</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>750</v>
+      </c>
+      <c r="B26" s="2">
+        <v>74.166666669999998</v>
+      </c>
+      <c r="C26" s="2">
+        <v>75.109672110000005</v>
+      </c>
+      <c r="D26" s="2">
+        <v>73.223661230000005</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.94300543969999995</v>
+      </c>
+      <c r="F26" s="2">
+        <v>75</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>750</v>
+      </c>
+      <c r="B27" s="2">
+        <v>75</v>
+      </c>
+      <c r="C27" s="2">
+        <v>75.943005439999993</v>
+      </c>
+      <c r="D27" s="2">
+        <v>74.056994560000007</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.94300543969999995</v>
+      </c>
+      <c r="F27" s="2">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>750</v>
+      </c>
+      <c r="B28" s="2">
+        <v>75.833333330000002</v>
+      </c>
+      <c r="C28" s="2">
+        <v>76.776338769999995</v>
+      </c>
+      <c r="D28" s="2">
+        <v>74.890327889999995</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.94300543969999995</v>
+      </c>
+      <c r="F28" s="2">
+        <v>75</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B29" s="2">
+        <v>82.5</v>
+      </c>
+      <c r="C29" s="2">
+        <v>83.443005439999993</v>
+      </c>
+      <c r="D29" s="2">
+        <v>81.556994560000007</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.94300543969999995</v>
+      </c>
+      <c r="F29" s="2">
+        <v>83.333333330000002</v>
+      </c>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B30" s="2">
+        <v>84.166666669999998</v>
+      </c>
+      <c r="C30" s="2">
+        <v>85.109672110000005</v>
+      </c>
+      <c r="D30" s="2">
+        <v>83.223661230000005</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.94300543969999995</v>
+      </c>
+      <c r="F30" s="2">
+        <v>83.333333330000002</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B31" s="2">
+        <v>83.333333330000002</v>
+      </c>
+      <c r="C31" s="2">
+        <v>84.276338769999995</v>
+      </c>
+      <c r="D31" s="2">
+        <v>82.390327889999995</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.94300543969999995</v>
+      </c>
+      <c r="F31" s="2">
+        <v>83.333333330000002</v>
+      </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B32" s="2">
+        <v>83.333333330000002</v>
+      </c>
+      <c r="C32" s="2">
+        <v>84.773797939999994</v>
+      </c>
+      <c r="D32" s="2">
+        <v>81.892868730000004</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F32" s="2">
+        <v>84.444444439999998</v>
+      </c>
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B33" s="2">
+        <v>85.833333330000002</v>
+      </c>
+      <c r="C33" s="2">
+        <v>87.273797939999994</v>
+      </c>
+      <c r="D33" s="2">
+        <v>84.392868730000004</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F33" s="2">
+        <v>84.444444439999998</v>
+      </c>
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B34" s="2">
+        <v>84.166666669999998</v>
+      </c>
+      <c r="C34" s="2">
+        <v>85.607131269999996</v>
+      </c>
+      <c r="D34" s="2">
+        <v>82.726202060000006</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1.4404646029999999</v>
+      </c>
+      <c r="F34" s="2">
+        <v>84.444444439999998</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B35" s="2">
+        <v>85.833333330000002</v>
+      </c>
+      <c r="C35" s="2">
+        <v>86.922222219999995</v>
+      </c>
+      <c r="D35" s="2">
+        <v>84.744444439999995</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F35" s="2">
+        <v>86.388888890000004</v>
+      </c>
+      <c r="G35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B36" s="2">
+        <v>85.833333330000002</v>
+      </c>
+      <c r="C36" s="2">
+        <v>86.922222219999995</v>
+      </c>
+      <c r="D36" s="2">
+        <v>84.744444439999995</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F36" s="2">
+        <v>86.388888890000004</v>
+      </c>
+      <c r="G36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B37" s="2">
+        <v>87.5</v>
+      </c>
+      <c r="C37" s="2">
+        <v>88.588888890000007</v>
+      </c>
+      <c r="D37" s="2">
+        <v>86.411111109999993</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F37" s="2">
+        <v>86.388888890000004</v>
+      </c>
+      <c r="G37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>300</v>
+      </c>
+      <c r="B38" s="2">
+        <v>53.333333330000002</v>
+      </c>
+      <c r="C38" s="2">
+        <v>54.422222220000002</v>
+      </c>
+      <c r="D38" s="2">
+        <v>52.244444440000002</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F38" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>300</v>
+      </c>
+      <c r="B39" s="2">
+        <v>51.666666669999998</v>
+      </c>
+      <c r="C39" s="2">
+        <v>52.755555559999998</v>
+      </c>
+      <c r="D39" s="2">
+        <v>50.577777779999998</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F39" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>300</v>
+      </c>
+      <c r="B40" s="2">
+        <v>53.333333330000002</v>
+      </c>
+      <c r="C40" s="2">
+        <v>54.422222220000002</v>
+      </c>
+      <c r="D40" s="2">
+        <v>52.244444440000002</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F40" s="2">
+        <v>52.777777780000001</v>
+      </c>
+      <c r="G40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>500</v>
+      </c>
+      <c r="B41" s="2">
+        <v>55.833333330000002</v>
+      </c>
+      <c r="C41" s="2">
+        <v>56.922222220000002</v>
+      </c>
+      <c r="D41" s="2">
+        <v>54.744444440000002</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F41" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>500</v>
+      </c>
+      <c r="B42" s="2">
+        <v>54.166666669999998</v>
+      </c>
+      <c r="C42" s="2">
+        <v>55.255555559999998</v>
+      </c>
+      <c r="D42" s="2">
+        <v>53.077777779999998</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F42" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>500</v>
+      </c>
+      <c r="B43" s="2">
+        <v>55.833333330000002</v>
+      </c>
+      <c r="C43" s="2">
+        <v>56.922222220000002</v>
+      </c>
+      <c r="D43" s="2">
+        <v>54.744444440000002</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F43" s="2">
+        <v>55.277777780000001</v>
+      </c>
+      <c r="G43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>750</v>
+      </c>
+      <c r="B44" s="2">
+        <v>66.666666669999998</v>
+      </c>
+      <c r="C44" s="2">
+        <v>68.629689029999994</v>
+      </c>
+      <c r="D44" s="2">
+        <v>64.703644310000001</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1.9630223609999999</v>
+      </c>
+      <c r="F44" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>750</v>
+      </c>
+      <c r="B45" s="2">
+        <v>64.166666669999998</v>
+      </c>
+      <c r="C45" s="2">
+        <v>66.129689029999994</v>
+      </c>
+      <c r="D45" s="2">
+        <v>62.203644310000001</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1.9630223609999999</v>
+      </c>
+      <c r="F45" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>750</v>
+      </c>
+      <c r="B46" s="2">
+        <v>63.333333330000002</v>
+      </c>
+      <c r="C46" s="2">
+        <v>65.296355689999999</v>
+      </c>
+      <c r="D46" s="2">
+        <v>61.370310969999998</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1.9630223609999999</v>
+      </c>
+      <c r="F46" s="2">
+        <v>64.722222220000006</v>
+      </c>
+      <c r="G46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B47" s="2">
+        <v>67.5</v>
+      </c>
+      <c r="C47" s="2">
+        <v>69.386010880000001</v>
+      </c>
+      <c r="D47" s="2">
+        <v>65.613989119999999</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1.8860108790000001</v>
+      </c>
+      <c r="F47" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="G47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B48" s="2">
+        <v>70.833333330000002</v>
+      </c>
+      <c r="C48" s="2">
+        <v>72.719344210000003</v>
+      </c>
+      <c r="D48" s="2">
+        <v>68.947322450000001</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1.8860108790000001</v>
+      </c>
+      <c r="F48" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="G48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B49" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="C49" s="2">
+        <v>71.052677549999999</v>
+      </c>
+      <c r="D49" s="2">
+        <v>67.280655789999997</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1.8860108790000001</v>
+      </c>
+      <c r="F49" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="G49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B50" s="2">
+        <v>69.166666669999998</v>
+      </c>
+      <c r="C50" s="2">
+        <v>71.539844979999998</v>
+      </c>
+      <c r="D50" s="2">
+        <v>66.793488350000004</v>
+      </c>
+      <c r="E50" s="2">
+        <v>2.373178314</v>
+      </c>
+      <c r="F50" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B51" s="2">
+        <v>70.833333330000002</v>
+      </c>
+      <c r="C51" s="2">
+        <v>73.206511649999996</v>
+      </c>
+      <c r="D51" s="2">
+        <v>68.460155020000002</v>
+      </c>
+      <c r="E51" s="2">
+        <v>2.373178314</v>
+      </c>
+      <c r="F51" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B52" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="C52" s="2">
+        <v>75.706511649999996</v>
+      </c>
+      <c r="D52" s="2">
+        <v>70.960155020000002</v>
+      </c>
+      <c r="E52" s="2">
+        <v>2.373178314</v>
+      </c>
+      <c r="F52" s="2">
+        <v>71.111111109999996</v>
+      </c>
+      <c r="G52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B53" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="C53" s="2">
+        <v>74.422222219999995</v>
+      </c>
+      <c r="D53" s="2">
+        <v>72.244444439999995</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F53" s="2">
+        <v>72.777777779999994</v>
+      </c>
+      <c r="G53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B54" s="2">
+        <v>73.333333330000002</v>
+      </c>
+      <c r="C54" s="2">
+        <v>74.422222219999995</v>
+      </c>
+      <c r="D54" s="2">
+        <v>72.244444439999995</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F54" s="2">
+        <v>72.777777779999994</v>
+      </c>
+      <c r="G54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B55" s="2">
+        <v>71.666666669999998</v>
+      </c>
+      <c r="C55" s="2">
+        <v>72.755555560000005</v>
+      </c>
+      <c r="D55" s="2">
+        <v>70.577777780000005</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1.0888888889999999</v>
+      </c>
+      <c r="F55" s="2">
+        <v>72.777777779999994</v>
+      </c>
+      <c r="G55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>